<commit_message>
predicted regular season standings
</commit_message>
<xml_diff>
--- a/Resources/sportsref_opp_21.xlsx
+++ b/Resources/sportsref_opp_21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99584ccd66595d1f/Documents/mathletics/NBA practice/nba21analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC3F57F9-804B-4DDA-A12F-28D21E8E567E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75B25CDA-ECC4-41FC-8138-AD4298BC347A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Rk</t>
   </si>
@@ -106,88 +106,85 @@
     <t>Phoenix Suns</t>
   </si>
   <si>
+    <t>Utah Jazz</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
     <t>Los Angeles Lakers</t>
   </si>
   <si>
-    <t>New York Knicks</t>
-  </si>
-  <si>
-    <t>Utah Jazz</t>
-  </si>
-  <si>
-    <t>Dallas Mavericks</t>
-  </si>
-  <si>
     <t>Milwaukee Bucks</t>
   </si>
   <si>
     <t>Indiana Pacers</t>
   </si>
   <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Los Angeles Clippers</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
     <t>Philadelphia 76ers</t>
   </si>
   <si>
-    <t>Miami Heat</t>
-  </si>
-  <si>
-    <t>Charlotte Hornets</t>
-  </si>
-  <si>
-    <t>Denver Nuggets</t>
-  </si>
-  <si>
-    <t>Atlanta Hawks</t>
-  </si>
-  <si>
-    <t>Houston Rockets</t>
-  </si>
-  <si>
-    <t>Detroit Pistons</t>
-  </si>
-  <si>
-    <t>Boston Celtics</t>
-  </si>
-  <si>
-    <t>Orlando Magic</t>
-  </si>
-  <si>
-    <t>Chicago Bulls</t>
-  </si>
-  <si>
-    <t>Cleveland Cavaliers</t>
-  </si>
-  <si>
-    <t>Oklahoma City Thunder</t>
-  </si>
-  <si>
-    <t>Toronto Raptors</t>
-  </si>
-  <si>
-    <t>Los Angeles Clippers</t>
+    <t>New Orleans Pelicans</t>
   </si>
   <si>
     <t>Portland Trail Blazers</t>
   </si>
   <si>
-    <t>New Orleans Pelicans</t>
-  </si>
-  <si>
     <t>Golden State Warriors</t>
   </si>
   <si>
     <t>Washington Wizards</t>
   </si>
   <si>
+    <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
     <t>Brooklyn Nets</t>
   </si>
   <si>
     <t>Sacramento Kings</t>
-  </si>
-  <si>
-    <t>Minnesota Timberwolves</t>
-  </si>
-  <si>
-    <t>League Average</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1144,25 +1143,25 @@
         <v>25</v>
       </c>
       <c r="C2" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2">
         <v>241.3</v>
       </c>
       <c r="E2" s="2">
-        <v>41.6</v>
+        <v>41.7</v>
       </c>
       <c r="F2" s="2">
-        <v>89.4</v>
+        <v>89.5</v>
       </c>
       <c r="G2" s="2">
-        <v>0.46500000000000002</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="H2" s="2">
         <v>12.7</v>
       </c>
       <c r="I2" s="2">
-        <v>33.799999999999997</v>
+        <v>33.9</v>
       </c>
       <c r="J2" s="2">
         <v>0.375</v>
@@ -1171,28 +1170,28 @@
         <v>29</v>
       </c>
       <c r="L2" s="2">
-        <v>55.7</v>
+        <v>55.6</v>
       </c>
       <c r="M2" s="2">
-        <v>0.52</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="N2" s="2">
         <v>14.2</v>
       </c>
       <c r="O2" s="2">
-        <v>19.2</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="P2" s="2">
-        <v>0.74</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="Q2" s="2">
-        <v>10.1</v>
+        <v>10</v>
       </c>
       <c r="R2" s="2">
-        <v>37.700000000000003</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="S2" s="2">
-        <v>47.8</v>
+        <v>47.9</v>
       </c>
       <c r="T2" s="2">
         <v>24.6</v>
@@ -1204,13 +1203,13 @@
         <v>5.4</v>
       </c>
       <c r="W2" s="2">
-        <v>13.9</v>
+        <v>13.8</v>
       </c>
       <c r="X2" s="2">
-        <v>18.399999999999999</v>
+        <v>18.3</v>
       </c>
       <c r="Y2" s="2">
-        <v>110.1</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1221,58 +1220,58 @@
         <v>26</v>
       </c>
       <c r="C3" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2">
-        <v>240.7</v>
+        <v>240.6</v>
       </c>
       <c r="E3" s="2">
-        <v>40.4</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="F3" s="2">
-        <v>85.8</v>
+        <v>85.9</v>
       </c>
       <c r="G3" s="2">
-        <v>0.47099999999999997</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H3" s="2">
         <v>13</v>
       </c>
       <c r="I3" s="2">
-        <v>34.9</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2">
-        <v>0.372</v>
+        <v>0.37</v>
       </c>
       <c r="K3" s="2">
-        <v>27.4</v>
+        <v>27.2</v>
       </c>
       <c r="L3" s="2">
-        <v>51</v>
+        <v>50.9</v>
       </c>
       <c r="M3" s="2">
-        <v>0.53800000000000003</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="N3" s="2">
-        <v>17.100000000000001</v>
+        <v>17.3</v>
       </c>
       <c r="O3" s="2">
-        <v>21.8</v>
+        <v>22.1</v>
       </c>
       <c r="P3" s="2">
-        <v>0.78200000000000003</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="Q3" s="2">
         <v>8.8000000000000007</v>
       </c>
       <c r="R3" s="2">
-        <v>34.9</v>
+        <v>35.1</v>
       </c>
       <c r="S3" s="2">
         <v>43.8</v>
       </c>
       <c r="T3" s="2">
-        <v>25.4</v>
+        <v>25.3</v>
       </c>
       <c r="U3" s="2">
         <v>8.1</v>
@@ -1281,13 +1280,13 @@
         <v>5.5</v>
       </c>
       <c r="W3" s="2">
-        <v>16.3</v>
+        <v>16.2</v>
       </c>
       <c r="X3" s="2">
-        <v>18.100000000000001</v>
+        <v>18.3</v>
       </c>
       <c r="Y3" s="2">
-        <v>110.8</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1298,46 +1297,46 @@
         <v>27</v>
       </c>
       <c r="C4" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
-        <v>242.5</v>
+        <v>242.4</v>
       </c>
       <c r="E4" s="2">
-        <v>39.9</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="F4" s="2">
         <v>86.7</v>
       </c>
       <c r="G4" s="2">
-        <v>0.46</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="H4" s="2">
-        <v>11.2</v>
+        <v>11</v>
       </c>
       <c r="I4" s="2">
-        <v>32.299999999999997</v>
+        <v>32.1</v>
       </c>
       <c r="J4" s="2">
-        <v>0.34699999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="K4" s="2">
         <v>28.7</v>
       </c>
       <c r="L4" s="2">
-        <v>54.5</v>
+        <v>54.6</v>
       </c>
       <c r="M4" s="2">
-        <v>0.52700000000000002</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="N4" s="2">
         <v>17</v>
       </c>
       <c r="O4" s="2">
-        <v>22.2</v>
+        <v>22.3</v>
       </c>
       <c r="P4" s="2">
-        <v>0.76500000000000001</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="Q4" s="2">
         <v>9.4</v>
@@ -1346,25 +1345,25 @@
         <v>33.5</v>
       </c>
       <c r="S4" s="2">
-        <v>43</v>
+        <v>42.9</v>
       </c>
       <c r="T4" s="2">
         <v>21.9</v>
       </c>
       <c r="U4" s="2">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="V4" s="2">
         <v>3.8</v>
       </c>
       <c r="W4" s="2">
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="X4" s="2">
         <v>18</v>
       </c>
       <c r="Y4" s="2">
-        <v>107.9</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1378,70 +1377,70 @@
         <v>41</v>
       </c>
       <c r="D5" s="2">
-        <v>243</v>
+        <v>240.6</v>
       </c>
       <c r="E5" s="2">
-        <v>40</v>
+        <v>41.5</v>
       </c>
       <c r="F5" s="2">
-        <v>88</v>
+        <v>91.4</v>
       </c>
       <c r="G5" s="2">
-        <v>0.45500000000000002</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="H5" s="2">
-        <v>11.6</v>
+        <v>11.1</v>
       </c>
       <c r="I5" s="2">
-        <v>32.799999999999997</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2">
-        <v>0.35299999999999998</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="K5" s="2">
-        <v>28.4</v>
+        <v>30.4</v>
       </c>
       <c r="L5" s="2">
-        <v>55.2</v>
+        <v>60.5</v>
       </c>
       <c r="M5" s="2">
-        <v>0.51500000000000001</v>
+        <v>0.502</v>
       </c>
       <c r="N5" s="2">
-        <v>14.7</v>
+        <v>14.9</v>
       </c>
       <c r="O5" s="2">
-        <v>19.399999999999999</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="P5" s="2">
-        <v>0.75800000000000001</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="Q5" s="2">
-        <v>8.8000000000000007</v>
+        <v>9.9</v>
       </c>
       <c r="R5" s="2">
         <v>32.5</v>
       </c>
       <c r="S5" s="2">
-        <v>41.2</v>
+        <v>42.4</v>
       </c>
       <c r="T5" s="2">
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="U5" s="2">
-        <v>8.1</v>
+        <v>7.5</v>
       </c>
       <c r="V5" s="2">
         <v>4.0999999999999996</v>
       </c>
       <c r="W5" s="2">
-        <v>14.9</v>
+        <v>11.7</v>
       </c>
       <c r="X5" s="2">
-        <v>21.6</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="Y5" s="2">
-        <v>106.3</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1452,10 +1451,10 @@
         <v>29</v>
       </c>
       <c r="C6" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
-        <v>240</v>
+        <v>240.6</v>
       </c>
       <c r="E6" s="2">
         <v>37.700000000000003</v>
@@ -1467,31 +1466,31 @@
         <v>0.442</v>
       </c>
       <c r="H6" s="2">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="I6" s="2">
-        <v>36.5</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="J6" s="2">
-        <v>0.33300000000000002</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="K6" s="2">
         <v>25.5</v>
       </c>
       <c r="L6" s="2">
-        <v>48.7</v>
+        <v>48.9</v>
       </c>
       <c r="M6" s="2">
-        <v>0.52300000000000002</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="N6" s="2">
-        <v>17.399999999999999</v>
+        <v>17.3</v>
       </c>
       <c r="O6" s="2">
         <v>22.5</v>
       </c>
       <c r="P6" s="2">
-        <v>0.77100000000000002</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="Q6" s="2">
         <v>9.3000000000000007</v>
@@ -1503,22 +1502,22 @@
         <v>43.6</v>
       </c>
       <c r="T6" s="2">
-        <v>22.9</v>
+        <v>22.8</v>
       </c>
       <c r="U6" s="2">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="V6" s="2">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="W6" s="2">
-        <v>12.1</v>
+        <v>12.3</v>
       </c>
       <c r="X6" s="2">
         <v>18.3</v>
       </c>
       <c r="Y6" s="2">
-        <v>104.9</v>
+        <v>104.8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1535,67 +1534,67 @@
         <v>240.6</v>
       </c>
       <c r="E7" s="2">
-        <v>41.5</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="F7" s="2">
-        <v>91.4</v>
+        <v>87.8</v>
       </c>
       <c r="G7" s="2">
-        <v>0.45300000000000001</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="H7" s="2">
-        <v>11.1</v>
+        <v>13.6</v>
       </c>
       <c r="I7" s="2">
-        <v>31</v>
+        <v>36.6</v>
       </c>
       <c r="J7" s="2">
-        <v>0.35799999999999998</v>
+        <v>0.371</v>
       </c>
       <c r="K7" s="2">
-        <v>30.4</v>
+        <v>26.8</v>
       </c>
       <c r="L7" s="2">
-        <v>60.5</v>
+        <v>51.2</v>
       </c>
       <c r="M7" s="2">
-        <v>0.502</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="N7" s="2">
-        <v>14.9</v>
+        <v>17</v>
       </c>
       <c r="O7" s="2">
-        <v>19.100000000000001</v>
+        <v>22.1</v>
       </c>
       <c r="P7" s="2">
-        <v>0.77600000000000002</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="Q7" s="2">
-        <v>9.9</v>
+        <v>10</v>
       </c>
       <c r="R7" s="2">
-        <v>32.5</v>
+        <v>34.6</v>
       </c>
       <c r="S7" s="2">
-        <v>42.4</v>
+        <v>44.6</v>
       </c>
       <c r="T7" s="2">
-        <v>22.5</v>
+        <v>22.9</v>
       </c>
       <c r="U7" s="2">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="V7" s="2">
-        <v>4.0999999999999996</v>
+        <v>3.6</v>
       </c>
       <c r="W7" s="2">
-        <v>11.7</v>
+        <v>12.7</v>
       </c>
       <c r="X7" s="2">
-        <v>19.899999999999999</v>
+        <v>20.6</v>
       </c>
       <c r="Y7" s="2">
-        <v>108.9</v>
+        <v>111.1</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1606,73 +1605,73 @@
         <v>31</v>
       </c>
       <c r="C8" s="2">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2">
+        <v>242.9</v>
+      </c>
+      <c r="E8" s="2">
         <v>40</v>
       </c>
-      <c r="D8" s="2">
-        <v>240.6</v>
-      </c>
-      <c r="E8" s="2">
-        <v>40.5</v>
-      </c>
       <c r="F8" s="2">
-        <v>87.8</v>
+        <v>88.2</v>
       </c>
       <c r="G8" s="2">
-        <v>0.46100000000000002</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="H8" s="2">
-        <v>13.7</v>
+        <v>11.6</v>
       </c>
       <c r="I8" s="2">
-        <v>36.5</v>
+        <v>32.9</v>
       </c>
       <c r="J8" s="2">
-        <v>0.375</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="K8" s="2">
-        <v>26.8</v>
+        <v>28.5</v>
       </c>
       <c r="L8" s="2">
-        <v>51.3</v>
+        <v>55.3</v>
       </c>
       <c r="M8" s="2">
-        <v>0.52200000000000002</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="N8" s="2">
-        <v>17</v>
+        <v>14.6</v>
       </c>
       <c r="O8" s="2">
-        <v>22.2</v>
+        <v>19.2</v>
       </c>
       <c r="P8" s="2">
-        <v>0.76600000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="Q8" s="2">
-        <v>10.1</v>
+        <v>9</v>
       </c>
       <c r="R8" s="2">
-        <v>34.799999999999997</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="S8" s="2">
-        <v>44.9</v>
+        <v>41.7</v>
       </c>
       <c r="T8" s="2">
-        <v>23</v>
+        <v>25.2</v>
       </c>
       <c r="U8" s="2">
-        <v>7.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="V8" s="2">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="W8" s="2">
-        <v>12.9</v>
+        <v>14.6</v>
       </c>
       <c r="X8" s="2">
-        <v>20.7</v>
+        <v>21.6</v>
       </c>
       <c r="Y8" s="2">
-        <v>111.6</v>
+        <v>106.2</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1683,49 +1682,49 @@
         <v>32</v>
       </c>
       <c r="C9" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>240.6</v>
       </c>
       <c r="E9" s="2">
-        <v>41.9</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2">
-        <v>92.2</v>
+        <v>92.3</v>
       </c>
       <c r="G9" s="2">
         <v>0.45400000000000001</v>
       </c>
       <c r="H9" s="2">
-        <v>14.2</v>
+        <v>14.1</v>
       </c>
       <c r="I9" s="2">
-        <v>37.9</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="J9" s="2">
         <v>0.374</v>
       </c>
       <c r="K9" s="2">
-        <v>27.7</v>
+        <v>27.8</v>
       </c>
       <c r="L9" s="2">
-        <v>54.3</v>
+        <v>54.5</v>
       </c>
       <c r="M9" s="2">
-        <v>0.50900000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="N9" s="2">
-        <v>14.6</v>
+        <v>14.4</v>
       </c>
       <c r="O9" s="2">
-        <v>18.7</v>
+        <v>18.5</v>
       </c>
       <c r="P9" s="2">
-        <v>0.77800000000000002</v>
+        <v>0.78</v>
       </c>
       <c r="Q9" s="2">
-        <v>9.4</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="R9" s="2">
         <v>34.200000000000003</v>
@@ -1734,7 +1733,7 @@
         <v>43.5</v>
       </c>
       <c r="T9" s="2">
-        <v>24.9</v>
+        <v>25</v>
       </c>
       <c r="U9" s="2">
         <v>6.8</v>
@@ -1743,10 +1742,10 @@
         <v>4.8</v>
       </c>
       <c r="W9" s="2">
-        <v>13.2</v>
+        <v>13</v>
       </c>
       <c r="X9" s="2">
-        <v>18.7</v>
+        <v>18.5</v>
       </c>
       <c r="Y9" s="2">
         <v>112.5</v>
@@ -1760,28 +1759,28 @@
         <v>33</v>
       </c>
       <c r="C10" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
-        <v>242.5</v>
+        <v>243</v>
       </c>
       <c r="E10" s="2">
-        <v>41.3</v>
+        <v>41.2</v>
       </c>
       <c r="F10" s="2">
-        <v>88.1</v>
+        <v>88.3</v>
       </c>
       <c r="G10" s="2">
-        <v>0.46899999999999997</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H10" s="2">
         <v>11.9</v>
       </c>
       <c r="I10" s="2">
-        <v>31.5</v>
+        <v>31.6</v>
       </c>
       <c r="J10" s="2">
-        <v>0.379</v>
+        <v>0.375</v>
       </c>
       <c r="K10" s="2">
         <v>29.4</v>
@@ -1799,19 +1798,19 @@
         <v>22.9</v>
       </c>
       <c r="P10" s="2">
-        <v>0.79800000000000004</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="Q10" s="2">
         <v>10.199999999999999</v>
       </c>
       <c r="R10" s="2">
-        <v>34.5</v>
+        <v>34.6</v>
       </c>
       <c r="S10" s="2">
-        <v>44.7</v>
+        <v>44.8</v>
       </c>
       <c r="T10" s="2">
-        <v>25.7</v>
+        <v>25.8</v>
       </c>
       <c r="U10" s="2">
         <v>7.5</v>
@@ -1826,7 +1825,7 @@
         <v>18.7</v>
       </c>
       <c r="Y10" s="2">
-        <v>112.8</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1837,73 +1836,73 @@
         <v>34</v>
       </c>
       <c r="C11" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2">
-        <v>242.4</v>
+        <v>242.3</v>
       </c>
       <c r="E11" s="2">
-        <v>40.200000000000003</v>
+        <v>38.6</v>
       </c>
       <c r="F11" s="2">
-        <v>89.4</v>
+        <v>87.1</v>
       </c>
       <c r="G11" s="2">
-        <v>0.45</v>
+        <v>0.443</v>
       </c>
       <c r="H11" s="2">
-        <v>12.3</v>
+        <v>14.7</v>
       </c>
       <c r="I11" s="2">
-        <v>34</v>
+        <v>40.6</v>
       </c>
       <c r="J11" s="2">
-        <v>0.36099999999999999</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="K11" s="2">
-        <v>28</v>
+        <v>23.9</v>
       </c>
       <c r="L11" s="2">
-        <v>55.4</v>
+        <v>46.6</v>
       </c>
       <c r="M11" s="2">
-        <v>0.504</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="N11" s="2">
-        <v>17.3</v>
+        <v>15.7</v>
       </c>
       <c r="O11" s="2">
-        <v>22.4</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="P11" s="2">
-        <v>0.77400000000000002</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="Q11" s="2">
-        <v>9.9</v>
+        <v>10.5</v>
       </c>
       <c r="R11" s="2">
-        <v>32.5</v>
+        <v>33.9</v>
       </c>
       <c r="S11" s="2">
-        <v>42.4</v>
+        <v>44.4</v>
       </c>
       <c r="T11" s="2">
-        <v>23.6</v>
+        <v>25.5</v>
       </c>
       <c r="U11" s="2">
-        <v>7.7</v>
+        <v>8.1</v>
       </c>
       <c r="V11" s="2">
-        <v>4.5999999999999996</v>
+        <v>4</v>
       </c>
       <c r="W11" s="2">
-        <v>15.2</v>
+        <v>15.3</v>
       </c>
       <c r="X11" s="2">
-        <v>21.2</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="Y11" s="2">
-        <v>110</v>
+        <v>107.6</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1917,70 +1916,70 @@
         <v>42</v>
       </c>
       <c r="D12" s="2">
-        <v>241.8</v>
+        <v>241.2</v>
       </c>
       <c r="E12" s="2">
-        <v>38.6</v>
+        <v>40.5</v>
       </c>
       <c r="F12" s="2">
-        <v>86.9</v>
+        <v>88.9</v>
       </c>
       <c r="G12" s="2">
-        <v>0.44500000000000001</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="H12" s="2">
-        <v>14.7</v>
+        <v>11.7</v>
       </c>
       <c r="I12" s="2">
-        <v>40.5</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="J12" s="2">
-        <v>0.36299999999999999</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="K12" s="2">
-        <v>23.9</v>
+        <v>28.8</v>
       </c>
       <c r="L12" s="2">
-        <v>46.4</v>
+        <v>55.1</v>
       </c>
       <c r="M12" s="2">
-        <v>0.51600000000000001</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="N12" s="2">
-        <v>15.6</v>
+        <v>17.8</v>
       </c>
       <c r="O12" s="2">
-        <v>19.899999999999999</v>
+        <v>22</v>
       </c>
       <c r="P12" s="2">
-        <v>0.78500000000000003</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="Q12" s="2">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="R12" s="2">
-        <v>33.9</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="S12" s="2">
-        <v>44.3</v>
+        <v>42.6</v>
       </c>
       <c r="T12" s="2">
-        <v>25.4</v>
+        <v>23.7</v>
       </c>
       <c r="U12" s="2">
-        <v>8.1</v>
+        <v>7.7</v>
       </c>
       <c r="V12" s="2">
-        <v>3.9</v>
+        <v>5.3</v>
       </c>
       <c r="W12" s="2">
-        <v>15.3</v>
+        <v>12.5</v>
       </c>
       <c r="X12" s="2">
-        <v>20.399999999999999</v>
+        <v>20.7</v>
       </c>
       <c r="Y12" s="2">
-        <v>107.5</v>
+        <v>110.5</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -1991,73 +1990,73 @@
         <v>36</v>
       </c>
       <c r="C13" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2">
-        <v>240.6</v>
+        <v>243.6</v>
       </c>
       <c r="E13" s="2">
+        <v>40.4</v>
+      </c>
+      <c r="F13" s="2">
+        <v>86.1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12.9</v>
+      </c>
+      <c r="I13" s="2">
+        <v>35.9</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="L13" s="2">
+        <v>50.2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="N13" s="2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="O13" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R13" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="S13" s="2">
         <v>41.9</v>
       </c>
-      <c r="F13" s="2">
-        <v>88.4</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="H13" s="2">
-        <v>15</v>
-      </c>
-      <c r="I13" s="2">
-        <v>40.5</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.371</v>
-      </c>
-      <c r="K13" s="2">
-        <v>26.9</v>
-      </c>
-      <c r="L13" s="2">
-        <v>47.9</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="N13" s="2">
-        <v>14.5</v>
-      </c>
-      <c r="O13" s="2">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>10.3</v>
-      </c>
-      <c r="R13" s="2">
-        <v>34.6</v>
-      </c>
-      <c r="S13" s="2">
-        <v>44.8</v>
-      </c>
       <c r="T13" s="2">
-        <v>28.3</v>
+        <v>26.6</v>
       </c>
       <c r="U13" s="2">
-        <v>8.3000000000000007</v>
+        <v>7.1</v>
       </c>
       <c r="V13" s="2">
-        <v>5.2</v>
+        <v>4.3</v>
       </c>
       <c r="W13" s="2">
-        <v>15.6</v>
+        <v>14.4</v>
       </c>
       <c r="X13" s="2">
-        <v>18.899999999999999</v>
+        <v>19.7</v>
       </c>
       <c r="Y13" s="2">
-        <v>113.2</v>
+        <v>110.7</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2071,70 +2070,70 @@
         <v>41</v>
       </c>
       <c r="D14" s="2">
-        <v>243.7</v>
+        <v>240.6</v>
       </c>
       <c r="E14" s="2">
-        <v>40.4</v>
+        <v>42</v>
       </c>
       <c r="F14" s="2">
-        <v>86.1</v>
+        <v>88.3</v>
       </c>
       <c r="G14" s="2">
-        <v>0.46899999999999997</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="H14" s="2">
-        <v>13</v>
+        <v>14.9</v>
       </c>
       <c r="I14" s="2">
-        <v>36</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="J14" s="2">
-        <v>0.36199999999999999</v>
+        <v>0.37</v>
       </c>
       <c r="K14" s="2">
-        <v>27.3</v>
+        <v>27</v>
       </c>
       <c r="L14" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M14" s="2">
-        <v>0.54600000000000004</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="N14" s="2">
-        <v>16.8</v>
+        <v>14.7</v>
       </c>
       <c r="O14" s="2">
-        <v>21.9</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="P14" s="2">
-        <v>0.76500000000000001</v>
+        <v>0.747</v>
       </c>
       <c r="Q14" s="2">
-        <v>9.6999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="R14" s="2">
-        <v>32.1</v>
+        <v>34.5</v>
       </c>
       <c r="S14" s="2">
-        <v>41.8</v>
+        <v>44.8</v>
       </c>
       <c r="T14" s="2">
-        <v>26.6</v>
+        <v>28.2</v>
       </c>
       <c r="U14" s="2">
-        <v>7.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="V14" s="2">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="W14" s="2">
-        <v>14.4</v>
+        <v>15.5</v>
       </c>
       <c r="X14" s="2">
-        <v>19.899999999999999</v>
+        <v>19</v>
       </c>
       <c r="Y14" s="2">
-        <v>110.6</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2145,73 +2144,73 @@
         <v>38</v>
       </c>
       <c r="C15" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2">
-        <v>241.2</v>
+        <v>240.6</v>
       </c>
       <c r="E15" s="2">
-        <v>40.700000000000003</v>
+        <v>39.6</v>
       </c>
       <c r="F15" s="2">
-        <v>89.1</v>
+        <v>85</v>
       </c>
       <c r="G15" s="2">
-        <v>0.45600000000000002</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="H15" s="2">
-        <v>11.8</v>
+        <v>12.6</v>
       </c>
       <c r="I15" s="2">
-        <v>34</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="J15" s="2">
-        <v>0.34599999999999997</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="K15" s="2">
-        <v>28.9</v>
+        <v>27</v>
       </c>
       <c r="L15" s="2">
-        <v>55.1</v>
+        <v>50.8</v>
       </c>
       <c r="M15" s="2">
-        <v>0.52500000000000002</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="N15" s="2">
-        <v>17.8</v>
+        <v>19</v>
       </c>
       <c r="O15" s="2">
-        <v>21.9</v>
+        <v>23.9</v>
       </c>
       <c r="P15" s="2">
-        <v>0.81399999999999995</v>
+        <v>0.79800000000000004</v>
       </c>
       <c r="Q15" s="2">
-        <v>10.4</v>
+        <v>9.4</v>
       </c>
       <c r="R15" s="2">
-        <v>32</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="S15" s="2">
-        <v>42.4</v>
+        <v>41.7</v>
       </c>
       <c r="T15" s="2">
-        <v>23.8</v>
+        <v>23.4</v>
       </c>
       <c r="U15" s="2">
-        <v>7.8</v>
+        <v>7.1</v>
       </c>
       <c r="V15" s="2">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="W15" s="2">
-        <v>12.4</v>
+        <v>14.2</v>
       </c>
       <c r="X15" s="2">
-        <v>20.8</v>
+        <v>19.7</v>
       </c>
       <c r="Y15" s="2">
-        <v>110.9</v>
+        <v>110.8</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2222,73 +2221,73 @@
         <v>39</v>
       </c>
       <c r="C16" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D16" s="2">
-        <v>240.6</v>
+        <v>243.6</v>
       </c>
       <c r="E16" s="2">
-        <v>41.4</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2">
-        <v>88.1</v>
+        <v>85.8</v>
       </c>
       <c r="G16" s="2">
-        <v>0.46899999999999997</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="H16" s="2">
-        <v>12.7</v>
+        <v>11.8</v>
       </c>
       <c r="I16" s="2">
-        <v>33.6</v>
+        <v>31.8</v>
       </c>
       <c r="J16" s="2">
-        <v>0.377</v>
+        <v>0.37</v>
       </c>
       <c r="K16" s="2">
-        <v>28.7</v>
+        <v>29.2</v>
       </c>
       <c r="L16" s="2">
-        <v>54.6</v>
+        <v>54</v>
       </c>
       <c r="M16" s="2">
-        <v>0.52600000000000002</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="N16" s="2">
-        <v>18.399999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="O16" s="2">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="P16" s="2">
-        <v>0.78300000000000003</v>
+        <v>0.76</v>
       </c>
       <c r="Q16" s="2">
         <v>9.8000000000000007</v>
       </c>
       <c r="R16" s="2">
-        <v>38.6</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="S16" s="2">
-        <v>48.4</v>
+        <v>44.6</v>
       </c>
       <c r="T16" s="2">
-        <v>24.2</v>
+        <v>25</v>
       </c>
       <c r="U16" s="2">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="V16" s="2">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
       <c r="W16" s="2">
-        <v>15.5</v>
+        <v>14.9</v>
       </c>
       <c r="X16" s="2">
-        <v>19.8</v>
+        <v>20.5</v>
       </c>
       <c r="Y16" s="2">
-        <v>113.7</v>
+        <v>110.8</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2302,70 +2301,70 @@
         <v>41</v>
       </c>
       <c r="D17" s="2">
-        <v>243.7</v>
+        <v>240.6</v>
       </c>
       <c r="E17" s="2">
-        <v>41.1</v>
+        <v>41.4</v>
       </c>
       <c r="F17" s="2">
-        <v>86</v>
+        <v>88.2</v>
       </c>
       <c r="G17" s="2">
-        <v>0.47799999999999998</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="H17" s="2">
-        <v>11.7</v>
+        <v>12.7</v>
       </c>
       <c r="I17" s="2">
-        <v>31.9</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="J17" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.376</v>
       </c>
       <c r="K17" s="2">
-        <v>29.4</v>
+        <v>28.7</v>
       </c>
       <c r="L17" s="2">
-        <v>54.1</v>
+        <v>54.5</v>
       </c>
       <c r="M17" s="2">
-        <v>0.54300000000000004</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="N17" s="2">
-        <v>17.2</v>
+        <v>18.3</v>
       </c>
       <c r="O17" s="2">
-        <v>22.7</v>
+        <v>23.5</v>
       </c>
       <c r="P17" s="2">
-        <v>0.75800000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="Q17" s="2">
-        <v>9.8000000000000007</v>
+        <v>10</v>
       </c>
       <c r="R17" s="2">
-        <v>34.6</v>
+        <v>38.5</v>
       </c>
       <c r="S17" s="2">
-        <v>44.4</v>
+        <v>48.5</v>
       </c>
       <c r="T17" s="2">
-        <v>24.9</v>
+        <v>24.1</v>
       </c>
       <c r="U17" s="2">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="V17" s="2">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="W17" s="2">
-        <v>14.8</v>
+        <v>15.6</v>
       </c>
       <c r="X17" s="2">
-        <v>20.5</v>
+        <v>19.8</v>
       </c>
       <c r="Y17" s="2">
-        <v>111.1</v>
+        <v>113.7</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2379,70 +2378,70 @@
         <v>41</v>
       </c>
       <c r="D18" s="2">
-        <v>240.6</v>
+        <v>242.4</v>
       </c>
       <c r="E18" s="2">
-        <v>39.799999999999997</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G18" s="2">
-        <v>0.46800000000000003</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="H18" s="2">
-        <v>12.6</v>
+        <v>11.2</v>
       </c>
       <c r="I18" s="2">
-        <v>34.299999999999997</v>
+        <v>32.5</v>
       </c>
       <c r="J18" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="K18" s="2">
-        <v>27.2</v>
+        <v>30.8</v>
       </c>
       <c r="L18" s="2">
-        <v>50.8</v>
+        <v>56.5</v>
       </c>
       <c r="M18" s="2">
-        <v>0.53500000000000003</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="N18" s="2">
-        <v>19</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="O18" s="2">
+        <v>24.1</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="R18" s="2">
+        <v>33.4</v>
+      </c>
+      <c r="S18" s="2">
+        <v>42.5</v>
+      </c>
+      <c r="T18" s="2">
         <v>23.7</v>
       </c>
-      <c r="P18" s="2">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>9.4</v>
-      </c>
-      <c r="R18" s="2">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="S18" s="2">
-        <v>41.6</v>
-      </c>
-      <c r="T18" s="2">
-        <v>23.5</v>
-      </c>
       <c r="U18" s="2">
-        <v>7.2</v>
+        <v>8.6</v>
       </c>
       <c r="V18" s="2">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="W18" s="2">
-        <v>14.4</v>
+        <v>13.6</v>
       </c>
       <c r="X18" s="2">
-        <v>19.899999999999999</v>
+        <v>18.8</v>
       </c>
       <c r="Y18" s="2">
-        <v>111.2</v>
+        <v>113.8</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2453,7 +2452,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2">
         <v>240.6</v>
@@ -2468,34 +2467,34 @@
         <v>0.46800000000000003</v>
       </c>
       <c r="H19" s="2">
-        <v>13.6</v>
+        <v>13.8</v>
       </c>
       <c r="I19" s="2">
-        <v>37.1</v>
+        <v>37.5</v>
       </c>
       <c r="J19" s="2">
-        <v>0.36599999999999999</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="K19" s="2">
-        <v>27.9</v>
+        <v>27.7</v>
       </c>
       <c r="L19" s="2">
-        <v>51.6</v>
+        <v>51.2</v>
       </c>
       <c r="M19" s="2">
         <v>0.54100000000000004</v>
       </c>
       <c r="N19" s="2">
-        <v>14.7</v>
+        <v>14.5</v>
       </c>
       <c r="O19" s="2">
-        <v>19</v>
+        <v>18.7</v>
       </c>
       <c r="P19" s="2">
-        <v>0.77400000000000002</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="Q19" s="2">
-        <v>8.8000000000000007</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="R19" s="2">
         <v>37.1</v>
@@ -2513,10 +2512,10 @@
         <v>5</v>
       </c>
       <c r="W19" s="2">
-        <v>12.7</v>
+        <v>12.6</v>
       </c>
       <c r="X19" s="2">
-        <v>18</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="Y19" s="2">
         <v>111.3</v>
@@ -2530,73 +2529,73 @@
         <v>43</v>
       </c>
       <c r="C20" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2">
-        <v>242.5</v>
+        <v>243</v>
       </c>
       <c r="E20" s="2">
-        <v>42.3</v>
+        <v>41.3</v>
       </c>
       <c r="F20" s="2">
-        <v>89.2</v>
+        <v>86.4</v>
       </c>
       <c r="G20" s="2">
-        <v>0.47399999999999998</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="H20" s="2">
-        <v>11.4</v>
+        <v>12.5</v>
       </c>
       <c r="I20" s="2">
-        <v>32.700000000000003</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="J20" s="2">
-        <v>0.34699999999999998</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="K20" s="2">
-        <v>30.9</v>
+        <v>28.7</v>
       </c>
       <c r="L20" s="2">
-        <v>56.5</v>
+        <v>54.2</v>
       </c>
       <c r="M20" s="2">
-        <v>0.54700000000000004</v>
+        <v>0.53</v>
       </c>
       <c r="N20" s="2">
-        <v>18.600000000000001</v>
+        <v>16.7</v>
       </c>
       <c r="O20" s="2">
-        <v>24.1</v>
+        <v>21.5</v>
       </c>
       <c r="P20" s="2">
-        <v>0.77200000000000002</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="Q20" s="2">
-        <v>9.1999999999999993</v>
+        <v>10.3</v>
       </c>
       <c r="R20" s="2">
-        <v>33.5</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="S20" s="2">
-        <v>42.7</v>
+        <v>43.5</v>
       </c>
       <c r="T20" s="2">
-        <v>23.8</v>
+        <v>24.2</v>
       </c>
       <c r="U20" s="2">
-        <v>8.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="V20" s="2">
-        <v>4.7</v>
+        <v>6</v>
       </c>
       <c r="W20" s="2">
-        <v>13.6</v>
+        <v>15.3</v>
       </c>
       <c r="X20" s="2">
-        <v>18.899999999999999</v>
+        <v>20.5</v>
       </c>
       <c r="Y20" s="2">
-        <v>114.5</v>
+        <v>111.8</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2607,73 +2606,73 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E21" s="2">
-        <v>41.4</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="F21" s="2">
-        <v>86.2</v>
+        <v>86.8</v>
       </c>
       <c r="G21" s="2">
-        <v>0.48</v>
+        <v>0.47</v>
       </c>
       <c r="H21" s="2">
-        <v>12.5</v>
+        <v>11.9</v>
       </c>
       <c r="I21" s="2">
-        <v>31.9</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="J21" s="2">
-        <v>0.39100000000000001</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="K21" s="2">
         <v>28.9</v>
       </c>
       <c r="L21" s="2">
-        <v>54.3</v>
+        <v>54</v>
       </c>
       <c r="M21" s="2">
-        <v>0.53200000000000003</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="N21" s="2">
-        <v>16.7</v>
+        <v>15.7</v>
       </c>
       <c r="O21" s="2">
-        <v>21.6</v>
+        <v>20.2</v>
       </c>
       <c r="P21" s="2">
-        <v>0.77400000000000002</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="Q21" s="2">
-        <v>10.4</v>
+        <v>8.9</v>
       </c>
       <c r="R21" s="2">
-        <v>33.299999999999997</v>
+        <v>32.4</v>
       </c>
       <c r="S21" s="2">
-        <v>43.7</v>
+        <v>41.2</v>
       </c>
       <c r="T21" s="2">
-        <v>24.3</v>
+        <v>23.4</v>
       </c>
       <c r="U21" s="2">
-        <v>8.6</v>
+        <v>7.2</v>
       </c>
       <c r="V21" s="2">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="W21" s="2">
-        <v>15.3</v>
+        <v>13.2</v>
       </c>
       <c r="X21" s="2">
-        <v>20.3</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="Y21" s="2">
-        <v>111.9</v>
+        <v>109.3</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2684,7 +2683,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2">
         <v>241.8</v>
@@ -2693,61 +2692,61 @@
         <v>42.4</v>
       </c>
       <c r="F22" s="2">
-        <v>91.2</v>
+        <v>90.9</v>
       </c>
       <c r="G22" s="2">
-        <v>0.46500000000000002</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="H22" s="2">
-        <v>12.6</v>
+        <v>12.7</v>
       </c>
       <c r="I22" s="2">
         <v>36.200000000000003</v>
       </c>
       <c r="J22" s="2">
-        <v>0.34899999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="K22" s="2">
-        <v>29.8</v>
+        <v>29.7</v>
       </c>
       <c r="L22" s="2">
-        <v>55</v>
+        <v>54.7</v>
       </c>
       <c r="M22" s="2">
-        <v>0.54200000000000004</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="N22" s="2">
-        <v>14.7</v>
+        <v>14.8</v>
       </c>
       <c r="O22" s="2">
-        <v>19.3</v>
+        <v>19.5</v>
       </c>
       <c r="P22" s="2">
-        <v>0.75900000000000001</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="Q22" s="2">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="R22" s="2">
-        <v>37.700000000000003</v>
+        <v>37.5</v>
       </c>
       <c r="S22" s="2">
-        <v>47.7</v>
+        <v>47.4</v>
       </c>
       <c r="T22" s="2">
-        <v>24.7</v>
+        <v>24.6</v>
       </c>
       <c r="U22" s="2">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="V22" s="2">
         <v>4.5999999999999996</v>
       </c>
       <c r="W22" s="2">
-        <v>13.1</v>
+        <v>13.2</v>
       </c>
       <c r="X22" s="2">
-        <v>18.3</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="Y22" s="2">
         <v>112.2</v>
@@ -2761,7 +2760,7 @@
         <v>46</v>
       </c>
       <c r="C23" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2">
         <v>240</v>
@@ -2770,64 +2769,64 @@
         <v>38.6</v>
       </c>
       <c r="F23" s="2">
-        <v>84.2</v>
+        <v>84</v>
       </c>
       <c r="G23" s="2">
-        <v>0.45900000000000002</v>
+        <v>0.46</v>
       </c>
       <c r="H23" s="2">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="I23" s="2">
-        <v>37.799999999999997</v>
+        <v>37.6</v>
       </c>
       <c r="J23" s="2">
-        <v>0.375</v>
+        <v>0.378</v>
       </c>
       <c r="K23" s="2">
-        <v>24.5</v>
+        <v>24.4</v>
       </c>
       <c r="L23" s="2">
-        <v>46.5</v>
+        <v>46.4</v>
       </c>
       <c r="M23" s="2">
-        <v>0.52700000000000002</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="N23" s="2">
         <v>20.8</v>
       </c>
       <c r="O23" s="2">
-        <v>26.1</v>
+        <v>26.2</v>
       </c>
       <c r="P23" s="2">
-        <v>0.79500000000000004</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="Q23" s="2">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="R23" s="2">
-        <v>35.9</v>
+        <v>36.1</v>
       </c>
       <c r="S23" s="2">
-        <v>45.8</v>
+        <v>46</v>
       </c>
       <c r="T23" s="2">
         <v>26.6</v>
       </c>
       <c r="U23" s="2">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="V23" s="2">
         <v>6</v>
       </c>
       <c r="W23" s="2">
-        <v>16.399999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="X23" s="2">
         <v>20.5</v>
       </c>
       <c r="Y23" s="2">
-        <v>112.2</v>
+        <v>112.3</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2838,73 +2837,73 @@
         <v>47</v>
       </c>
       <c r="C24" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2">
-        <v>240</v>
+        <v>242.9</v>
       </c>
       <c r="E24" s="2">
-        <v>41</v>
+        <v>40.1</v>
       </c>
       <c r="F24" s="2">
-        <v>86.9</v>
+        <v>89.3</v>
       </c>
       <c r="G24" s="2">
-        <v>0.47199999999999998</v>
+        <v>0.45</v>
       </c>
       <c r="H24" s="2">
-        <v>11.9</v>
+        <v>12.2</v>
       </c>
       <c r="I24" s="2">
-        <v>32.6</v>
+        <v>33.6</v>
       </c>
       <c r="J24" s="2">
-        <v>0.36399999999999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="K24" s="2">
-        <v>29.2</v>
+        <v>28</v>
       </c>
       <c r="L24" s="2">
-        <v>54.4</v>
+        <v>55.7</v>
       </c>
       <c r="M24" s="2">
-        <v>0.53700000000000003</v>
+        <v>0.502</v>
       </c>
       <c r="N24" s="2">
-        <v>15.6</v>
+        <v>17.2</v>
       </c>
       <c r="O24" s="2">
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="P24" s="2">
-        <v>0.78</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="Q24" s="2">
-        <v>8.8000000000000007</v>
+        <v>9.9</v>
       </c>
       <c r="R24" s="2">
-        <v>32.5</v>
+        <v>32.4</v>
       </c>
       <c r="S24" s="2">
-        <v>41.3</v>
+        <v>42.3</v>
       </c>
       <c r="T24" s="2">
-        <v>23.4</v>
+        <v>23.5</v>
       </c>
       <c r="U24" s="2">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="V24" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="W24" s="2">
-        <v>13.1</v>
+        <v>15.1</v>
       </c>
       <c r="X24" s="2">
-        <v>17.899999999999999</v>
+        <v>21.2</v>
       </c>
       <c r="Y24" s="2">
-        <v>109.6</v>
+        <v>109.7</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2915,73 +2914,73 @@
         <v>48</v>
       </c>
       <c r="C25" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2">
-        <v>240.6</v>
+        <v>241.2</v>
       </c>
       <c r="E25" s="2">
-        <v>42</v>
+        <v>41.7</v>
       </c>
       <c r="F25" s="2">
-        <v>87.8</v>
+        <v>88.1</v>
       </c>
       <c r="G25" s="2">
-        <v>0.47799999999999998</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="H25" s="2">
+        <v>15.4</v>
+      </c>
+      <c r="I25" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="K25" s="2">
+        <v>26.3</v>
+      </c>
+      <c r="L25" s="2">
+        <v>48.6</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="N25" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="O25" s="2">
+        <v>20.3</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="R25" s="2">
+        <v>31.4</v>
+      </c>
+      <c r="S25" s="2">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="T25" s="2">
+        <v>26.7</v>
+      </c>
+      <c r="U25" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="V25" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="W25" s="2">
         <v>13</v>
       </c>
-      <c r="I25" s="2">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.374</v>
-      </c>
-      <c r="K25" s="2">
-        <v>29</v>
-      </c>
-      <c r="L25" s="2">
-        <v>53</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="N25" s="2">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="O25" s="2">
-        <v>23.4</v>
-      </c>
-      <c r="P25" s="2">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>10.3</v>
-      </c>
-      <c r="R25" s="2">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="S25" s="2">
-        <v>46.1</v>
-      </c>
-      <c r="T25" s="2">
-        <v>25.3</v>
-      </c>
-      <c r="U25" s="2">
-        <v>6.3</v>
-      </c>
-      <c r="V25" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="W25" s="2">
-        <v>12.8</v>
-      </c>
       <c r="X25" s="2">
-        <v>18.7</v>
+        <v>20.9</v>
       </c>
       <c r="Y25" s="2">
-        <v>115.1</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -2992,73 +2991,73 @@
         <v>49</v>
       </c>
       <c r="C26" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2">
-        <v>241.2</v>
+        <v>240.6</v>
       </c>
       <c r="E26" s="2">
-        <v>41.6</v>
+        <v>42.1</v>
       </c>
       <c r="F26" s="2">
-        <v>88.1</v>
+        <v>87.7</v>
       </c>
       <c r="G26" s="2">
-        <v>0.47299999999999998</v>
+        <v>0.48</v>
       </c>
       <c r="H26" s="2">
-        <v>15.4</v>
+        <v>13.2</v>
       </c>
       <c r="I26" s="2">
-        <v>39.6</v>
+        <v>34.9</v>
       </c>
       <c r="J26" s="2">
-        <v>0.39</v>
+        <v>0.378</v>
       </c>
       <c r="K26" s="2">
-        <v>26.2</v>
+        <v>29</v>
       </c>
       <c r="L26" s="2">
-        <v>48.5</v>
+        <v>52.9</v>
       </c>
       <c r="M26" s="2">
-        <v>0.54100000000000004</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="N26" s="2">
-        <v>16.7</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="O26" s="2">
-        <v>20.6</v>
+        <v>23.3</v>
       </c>
       <c r="P26" s="2">
-        <v>0.81</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="Q26" s="2">
-        <v>8.6999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="R26" s="2">
-        <v>31.5</v>
+        <v>36</v>
       </c>
       <c r="S26" s="2">
-        <v>40.200000000000003</v>
+        <v>46.2</v>
       </c>
       <c r="T26" s="2">
-        <v>26.6</v>
+        <v>25.2</v>
       </c>
       <c r="U26" s="2">
-        <v>7.4</v>
+        <v>6.3</v>
       </c>
       <c r="V26" s="2">
-        <v>5.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W26" s="2">
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="X26" s="2">
-        <v>20.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="Y26" s="2">
-        <v>115.4</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -3069,70 +3068,70 @@
         <v>50</v>
       </c>
       <c r="C27" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2">
         <v>240.6</v>
       </c>
       <c r="E27" s="2">
-        <v>39.9</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="F27" s="2">
-        <v>89.2</v>
+        <v>89.3</v>
       </c>
       <c r="G27" s="2">
-        <v>0.44700000000000001</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="H27" s="2">
         <v>13</v>
       </c>
       <c r="I27" s="2">
-        <v>35.299999999999997</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="J27" s="2">
-        <v>0.36899999999999999</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="K27" s="2">
         <v>26.9</v>
       </c>
       <c r="L27" s="2">
-        <v>54</v>
+        <v>54.2</v>
       </c>
       <c r="M27" s="2">
-        <v>0.498</v>
+        <v>0.496</v>
       </c>
       <c r="N27" s="2">
-        <v>20.3</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="O27" s="2">
-        <v>26.1</v>
+        <v>26.2</v>
       </c>
       <c r="P27" s="2">
-        <v>0.77800000000000002</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="Q27" s="2">
         <v>11</v>
       </c>
       <c r="R27" s="2">
-        <v>37.5</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="S27" s="2">
-        <v>48.5</v>
+        <v>48.7</v>
       </c>
       <c r="T27" s="2">
         <v>23.7</v>
       </c>
       <c r="U27" s="2">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="V27" s="2">
         <v>4.8</v>
       </c>
       <c r="W27" s="2">
-        <v>15.8</v>
+        <v>15.7</v>
       </c>
       <c r="X27" s="2">
-        <v>20.399999999999999</v>
+        <v>20.5</v>
       </c>
       <c r="Y27" s="2">
         <v>113.1</v>
@@ -3146,7 +3145,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2">
         <v>240.6</v>
@@ -3161,58 +3160,58 @@
         <v>0.47599999999999998</v>
       </c>
       <c r="H28" s="2">
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="I28" s="2">
-        <v>34.799999999999997</v>
+        <v>34.6</v>
       </c>
       <c r="J28" s="2">
-        <v>0.38400000000000001</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="K28" s="2">
-        <v>30</v>
+        <v>30.1</v>
       </c>
       <c r="L28" s="2">
-        <v>56.3</v>
+        <v>56.4</v>
       </c>
       <c r="M28" s="2">
-        <v>0.53300000000000003</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="N28" s="2">
-        <v>20.2</v>
+        <v>20</v>
       </c>
       <c r="O28" s="2">
-        <v>25.9</v>
+        <v>25.8</v>
       </c>
       <c r="P28" s="2">
-        <v>0.77700000000000002</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="Q28" s="2">
-        <v>10.3</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="R28" s="2">
-        <v>37.200000000000003</v>
+        <v>36.9</v>
       </c>
       <c r="S28" s="2">
-        <v>47.4</v>
+        <v>47.1</v>
       </c>
       <c r="T28" s="2">
         <v>24.4</v>
       </c>
       <c r="U28" s="2">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="V28" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="W28" s="2">
-        <v>15.2</v>
+        <v>15</v>
       </c>
       <c r="X28" s="2">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="Y28" s="2">
-        <v>120.2</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -3226,70 +3225,70 @@
         <v>42</v>
       </c>
       <c r="D29" s="2">
-        <v>243</v>
+        <v>241.8</v>
       </c>
       <c r="E29" s="2">
         <v>43</v>
       </c>
       <c r="F29" s="2">
-        <v>92.5</v>
+        <v>89.5</v>
       </c>
       <c r="G29" s="2">
-        <v>0.46600000000000003</v>
+        <v>0.48</v>
       </c>
       <c r="H29" s="2">
-        <v>12.9</v>
+        <v>11.8</v>
       </c>
       <c r="I29" s="2">
-        <v>35.299999999999997</v>
+        <v>31.2</v>
       </c>
       <c r="J29" s="2">
-        <v>0.36499999999999999</v>
+        <v>0.379</v>
       </c>
       <c r="K29" s="2">
-        <v>30.1</v>
+        <v>31.1</v>
       </c>
       <c r="L29" s="2">
-        <v>57.1</v>
+        <v>58.2</v>
       </c>
       <c r="M29" s="2">
-        <v>0.52800000000000002</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="N29" s="2">
-        <v>16.399999999999999</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="O29" s="2">
-        <v>21.1</v>
+        <v>24.5</v>
       </c>
       <c r="P29" s="2">
-        <v>0.77700000000000002</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="Q29" s="2">
-        <v>10</v>
+        <v>10.4</v>
       </c>
       <c r="R29" s="2">
-        <v>32.200000000000003</v>
+        <v>36.4</v>
       </c>
       <c r="S29" s="2">
-        <v>42.2</v>
+        <v>46.8</v>
       </c>
       <c r="T29" s="2">
-        <v>24.7</v>
+        <v>26.2</v>
       </c>
       <c r="U29" s="2">
-        <v>7.9</v>
+        <v>7.4</v>
       </c>
       <c r="V29" s="2">
-        <v>4.4000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="W29" s="2">
-        <v>12.6</v>
+        <v>15.2</v>
       </c>
       <c r="X29" s="2">
-        <v>18.7</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="Y29" s="2">
-        <v>115.4</v>
+        <v>117.2</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -3300,73 +3299,73 @@
         <v>53</v>
       </c>
       <c r="C30" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2">
-        <v>240.6</v>
+        <v>242.9</v>
       </c>
       <c r="E30" s="2">
-        <v>44.3</v>
+        <v>43</v>
       </c>
       <c r="F30" s="2">
-        <v>90.5</v>
+        <v>92.1</v>
       </c>
       <c r="G30" s="2">
-        <v>0.48899999999999999</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H30" s="2">
-        <v>13.1</v>
+        <v>12.8</v>
       </c>
       <c r="I30" s="2">
-        <v>33.4</v>
+        <v>35</v>
       </c>
       <c r="J30" s="2">
-        <v>0.39200000000000002</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="K30" s="2">
-        <v>31.2</v>
+        <v>30.3</v>
       </c>
       <c r="L30" s="2">
         <v>57.2</v>
       </c>
       <c r="M30" s="2">
-        <v>0.54600000000000004</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="N30" s="2">
-        <v>17.8</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="O30" s="2">
-        <v>22.1</v>
+        <v>21.1</v>
       </c>
       <c r="P30" s="2">
-        <v>0.80400000000000005</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="Q30" s="2">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="R30" s="2">
-        <v>34.200000000000003</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="S30" s="2">
-        <v>44.7</v>
+        <v>42.3</v>
       </c>
       <c r="T30" s="2">
-        <v>26</v>
+        <v>24.7</v>
       </c>
       <c r="U30" s="2">
-        <v>7.4</v>
+        <v>7.8</v>
       </c>
       <c r="V30" s="2">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W30" s="2">
-        <v>13</v>
+        <v>12.7</v>
       </c>
       <c r="X30" s="2">
-        <v>20</v>
+        <v>18.8</v>
       </c>
       <c r="Y30" s="2">
-        <v>119.4</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
@@ -3380,147 +3379,73 @@
         <v>42</v>
       </c>
       <c r="D31" s="2">
-        <v>241.8</v>
+        <v>240.6</v>
       </c>
       <c r="E31" s="2">
-        <v>43</v>
+        <v>44.4</v>
       </c>
       <c r="F31" s="2">
-        <v>89.5</v>
+        <v>90.4</v>
       </c>
       <c r="G31" s="2">
-        <v>0.48</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="H31" s="2">
-        <v>11.8</v>
+        <v>13</v>
       </c>
       <c r="I31" s="2">
-        <v>31.2</v>
+        <v>33.1</v>
       </c>
       <c r="J31" s="2">
-        <v>0.379</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="K31" s="2">
-        <v>31.1</v>
+        <v>31.4</v>
       </c>
       <c r="L31" s="2">
-        <v>58.2</v>
+        <v>57.3</v>
       </c>
       <c r="M31" s="2">
-        <v>0.53500000000000003</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="N31" s="2">
-        <v>19.399999999999999</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="O31" s="2">
-        <v>24.5</v>
+        <v>22.3</v>
       </c>
       <c r="P31" s="2">
-        <v>0.79100000000000004</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="Q31" s="2">
         <v>10.4</v>
       </c>
       <c r="R31" s="2">
-        <v>36.4</v>
+        <v>34.4</v>
       </c>
       <c r="S31" s="2">
-        <v>46.8</v>
+        <v>44.8</v>
       </c>
       <c r="T31" s="2">
-        <v>26.2</v>
+        <v>25.9</v>
       </c>
       <c r="U31" s="2">
         <v>7.4</v>
       </c>
       <c r="V31" s="2">
-        <v>5.5</v>
+        <v>4.7</v>
       </c>
       <c r="W31" s="2">
-        <v>15.2</v>
+        <v>12.9</v>
       </c>
       <c r="X31" s="2">
-        <v>18.899999999999999</v>
+        <v>20</v>
       </c>
       <c r="Y31" s="2">
-        <v>117.2</v>
+        <v>119.6</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="2">
-        <v>41</v>
-      </c>
-      <c r="D32" s="2">
-        <v>241.4</v>
-      </c>
-      <c r="E32" s="2">
-        <v>41.1</v>
-      </c>
-      <c r="F32" s="2">
-        <v>88.3</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="H32" s="2">
-        <v>12.8</v>
-      </c>
-      <c r="I32" s="2">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="K32" s="2">
-        <v>28.3</v>
-      </c>
-      <c r="L32" s="2">
-        <v>53.5</v>
-      </c>
-      <c r="M32" s="2">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="N32" s="2">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="O32" s="2">
-        <v>21.9</v>
-      </c>
-      <c r="P32" s="2">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="R32" s="2">
-        <v>34.5</v>
-      </c>
-      <c r="S32" s="2">
-        <v>44.3</v>
-      </c>
-      <c r="T32" s="2">
-        <v>24.7</v>
-      </c>
-      <c r="U32" s="2">
-        <v>7.6</v>
-      </c>
-      <c r="V32" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="W32" s="2">
-        <v>14.1</v>
-      </c>
-      <c r="X32" s="2">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="Y32" s="2">
-        <v>112</v>
-      </c>
-    </row>
+    <row r="32" spans="1:25" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>